<commit_message>
Getting rows and it's cells from sheet
</commit_message>
<xml_diff>
--- a/Test Data/Test Data.xlsx
+++ b/Test Data/Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Career\My Projects\Selenium Projects\06-Selenium-Excel-Data-Driven-Testing-Functions\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Career\My Projects\Selenium Projects\06-Selenium-Excel-Data-Driven-Testing-Functions\ExcelDriven\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6539FF-B961-41A4-B053-2E24AA98883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BC4023-6210-4055-AE57-1E98AF074507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{A4EE1558-29D8-42C8-BA9C-FF0A8DCD568E}"/>
+    <workbookView xWindow="2535" yWindow="1935" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{A4EE1558-29D8-42C8-BA9C-FF0A8DCD568E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -810,6 +810,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="441aac4b-6dfc-4194-bb8a-160ce77cf504" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E8C09F421E528479928880B7919B6C2" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="196b63fa03bc726e59bebe6ae52dbc1a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="441aac4b-6dfc-4194-bb8a-160ce77cf504" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79ea872b03c10337295506efc728ac24" ns3:_="">
     <xsd:import namespace="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
@@ -965,24 +982,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="441aac4b-6dfc-4194-bb8a-160ce77cf504" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D5DF8E-87F1-4867-8661-99EFFF494E55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38087219-72F9-464A-BEA7-789EB56B72FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A81BAEA9-ED83-4854-AA05-9CDD09A130DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -998,28 +1022,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38087219-72F9-464A-BEA7-789EB56B72FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D5DF8E-87F1-4867-8661-99EFFF494E55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Retrieving data from excel based on condition
</commit_message>
<xml_diff>
--- a/Test Data/Test Data.xlsx
+++ b/Test Data/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Career\My Projects\Selenium Projects\06-Selenium-Excel-Data-Driven-Testing-Functions\ExcelDriven\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BC4023-6210-4055-AE57-1E98AF074507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC408CF5-A35A-406F-A9C5-20CA95ABEB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="1935" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{A4EE1558-29D8-42C8-BA9C-FF0A8DCD568E}"/>
+    <workbookView xWindow="2535" yWindow="1935" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A4EE1558-29D8-42C8-BA9C-FF0A8DCD568E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393DB358-5CDA-4B3D-824B-E4347D1EC0DF}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4449F26-0F6B-4AAE-8A3B-1A5C43FA099D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Practise exercise - excel driven testing - 1
</commit_message>
<xml_diff>
--- a/Test Data/Test Data.xlsx
+++ b/Test Data/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Career\My Projects\Selenium Projects\06-Selenium-Excel-Data-Driven-Testing-Functions\ExcelDriven\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC408CF5-A35A-406F-A9C5-20CA95ABEB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E143199C-1003-4947-9A5C-15E3F720B43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="1935" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A4EE1558-29D8-42C8-BA9C-FF0A8DCD568E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A4EE1558-29D8-42C8-BA9C-FF0A8DCD568E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -634,7 +634,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,23 +810,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="441aac4b-6dfc-4194-bb8a-160ce77cf504" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E8C09F421E528479928880B7919B6C2" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="196b63fa03bc726e59bebe6ae52dbc1a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="441aac4b-6dfc-4194-bb8a-160ce77cf504" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79ea872b03c10337295506efc728ac24" ns3:_="">
     <xsd:import namespace="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
@@ -982,31 +965,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="441aac4b-6dfc-4194-bb8a-160ce77cf504" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D5DF8E-87F1-4867-8661-99EFFF494E55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38087219-72F9-464A-BEA7-789EB56B72FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A81BAEA9-ED83-4854-AA05-9CDD09A130DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1022,4 +998,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38087219-72F9-464A-BEA7-789EB56B72FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D5DF8E-87F1-4867-8661-99EFFF494E55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Integrating excel to dataprovider to parameterized data
</commit_message>
<xml_diff>
--- a/Test Data/Test Data.xlsx
+++ b/Test Data/Test Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Career\My Projects\Selenium Projects\06-Selenium-Excel-Data-Driven-Testing-Functions\ExcelDriven\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E143199C-1003-4947-9A5C-15E3F720B43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2160D0-FCC5-49B7-A3FD-618017F6C2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A4EE1558-29D8-42C8-BA9C-FF0A8DCD568E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{A4EE1558-29D8-42C8-BA9C-FF0A8DCD568E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Test Cases</t>
   </si>
@@ -170,6 +171,33 @@
   </si>
   <si>
     <t>S3 Test Delete 3</t>
+  </si>
+  <si>
+    <t>Hello1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text2 </t>
+  </si>
+  <si>
+    <t>Param1</t>
+  </si>
+  <si>
+    <t>Param2</t>
+  </si>
+  <si>
+    <t>Param3</t>
+  </si>
+  <si>
+    <t>Text1</t>
   </si>
 </sst>
 </file>
@@ -205,8 +233,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393DB358-5CDA-4B3D-824B-E4347D1EC0DF}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -809,7 +840,88 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C60B10-72FA-4BEB-9CDD-9AA89F69D77A}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="441aac4b-6dfc-4194-bb8a-160ce77cf504" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E8C09F421E528479928880B7919B6C2" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="196b63fa03bc726e59bebe6ae52dbc1a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="441aac4b-6dfc-4194-bb8a-160ce77cf504" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79ea872b03c10337295506efc728ac24" ns3:_="">
     <xsd:import namespace="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
@@ -965,24 +1077,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="441aac4b-6dfc-4194-bb8a-160ce77cf504" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D5DF8E-87F1-4867-8661-99EFFF494E55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38087219-72F9-464A-BEA7-789EB56B72FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A81BAEA9-ED83-4854-AA05-9CDD09A130DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -998,28 +1117,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38087219-72F9-464A-BEA7-789EB56B72FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D5DF8E-87F1-4867-8661-99EFFF494E55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="441aac4b-6dfc-4194-bb8a-160ce77cf504"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>